<commit_message>
Deploying to gh-pages from @ cakeoclock/cakeoclock.github.io@5298aff69fb891cc7be6350185250b19be0be5f0 🚀
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amit/Projects/cake-o-clock/public/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amit/Projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1D0FB4-CE92-8A4B-9CC3-4051CCA09E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73460C8A-5742-AA4A-B667-00C71DDE1A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -624,7 +624,7 @@
   <dimension ref="A1:AC13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -990,7 +990,7 @@
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ cakeoclock/cakeoclock.github.io@a3613b101947681758d6bb94b97dc4dff5d5e2eb 🚀
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amit/Projects/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73460C8A-5742-AA4A-B667-00C71DDE1A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="504" windowWidth="16608" windowHeight="9432" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cream Cakes" sheetId="1" r:id="rId1"/>
@@ -18,7 +12,7 @@
     <sheet name="Pastries" sheetId="3" r:id="rId3"/>
     <sheet name="Sweet Delights" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -349,8 +343,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -617,25 +611,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="25.83203125" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
     <col min="5" max="5" width="22.6640625" customWidth="1"/>
     <col min="6" max="6" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -686,7 +680,7 @@
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
     </row>
-    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:29" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -712,7 +706,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:29" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -738,7 +732,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:29" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -764,7 +758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:29" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -790,7 +784,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:29" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -816,7 +810,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:29" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
@@ -842,7 +836,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:29" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -868,7 +862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:29" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
@@ -894,7 +888,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:29" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
@@ -920,7 +914,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:29" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>40</v>
       </c>
@@ -946,7 +940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:29" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
@@ -972,7 +966,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:29" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>46</v>
       </c>
@@ -990,7 +984,7 @@
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>15</v>
@@ -998,13 +992,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:H13" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:H13">
       <formula1>"yes,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E12" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E12">
       <formula1>"For every 500 gm,Per Piece"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E13" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E13">
       <formula1>"For every 500 gm,Per Piece,For 1 kg"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1013,7 +1007,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1023,13 +1017,13 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1080,7 +1074,7 @@
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
     </row>
-    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:29" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
@@ -1106,7 +1100,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:29" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>53</v>
       </c>
@@ -1132,7 +1126,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:29" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>56</v>
       </c>
@@ -1160,10 +1154,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:H4" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:H4">
       <formula1>"yes,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E4">
       <formula1>"For every 500 gm,Per Piece"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1172,7 +1166,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1182,12 +1176,12 @@
       <selection activeCell="F2" sqref="F2:F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1238,7 +1232,7 @@
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
     </row>
-    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:29" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>59</v>
       </c>
@@ -1262,7 +1256,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:29" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>63</v>
       </c>
@@ -1286,7 +1280,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:29" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>66</v>
       </c>
@@ -1310,7 +1304,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:29" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>69</v>
       </c>
@@ -1334,7 +1328,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:29" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>72</v>
       </c>
@@ -1358,7 +1352,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:29" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>75</v>
       </c>
@@ -1382,7 +1376,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:29" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>78</v>
       </c>
@@ -1406,7 +1400,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:29" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>81</v>
       </c>
@@ -1432,10 +1426,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:H9" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:H9">
       <formula1>"yes,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E9" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E9">
       <formula1>"For every 500 gm,Per Piece"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1444,22 +1438,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="3" max="3" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1510,7 +1504,7 @@
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
     </row>
-    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:29" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>84</v>
       </c>
@@ -1534,7 +1528,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:29" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>87</v>
       </c>
@@ -1558,7 +1552,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:29" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>90</v>
       </c>
@@ -1584,10 +1578,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:H4" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:H4">
       <formula1>"yes,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E4">
       <formula1>"For every 500 gm,Per Piece"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ cakeoclock/cakeoclock.github.io@953585556663c7a0e2bd4f7314a71972e482f16e 🚀
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="504" windowWidth="16608" windowHeight="9432" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="504" windowWidth="16608" windowHeight="9432"/>
   </bookViews>
   <sheets>
     <sheet name="Cream Cakes" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="108">
   <si>
     <t>id</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>Representing the sweetness and joy of life, this cake is one of the favourites of children and has rich flavours of strawberry.</t>
+  </si>
+  <si>
+    <t>price charged according to flavour</t>
   </si>
 </sst>
 </file>
@@ -617,8 +620,8 @@
   </sheetPr>
   <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -691,7 +694,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="2">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
@@ -743,7 +746,7 @@
         <v>21</v>
       </c>
       <c r="D4" s="2">
-        <v>380</v>
+        <v>350</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -847,7 +850,7 @@
         <v>33</v>
       </c>
       <c r="D8" s="2">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>13</v>
@@ -873,7 +876,7 @@
         <v>36</v>
       </c>
       <c r="D9" s="2">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>13</v>
@@ -899,7 +902,7 @@
         <v>39</v>
       </c>
       <c r="D10" s="2">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>13</v>
@@ -925,7 +928,7 @@
         <v>42</v>
       </c>
       <c r="D11" s="2">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>13</v>
@@ -951,7 +954,7 @@
         <v>45</v>
       </c>
       <c r="D12" s="2">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>13</v>
@@ -982,7 +985,9 @@
       <c r="E13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="G13" s="2" t="s">
         <v>14</v>
       </c>
@@ -1444,7 +1449,7 @@
   </sheetPr>
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ cakeoclock/cakeoclock.github.io@02e2a4d658cbc6211d5af08fb94f2adf7f9c8092 🚀
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="504" windowWidth="16608" windowHeight="9432"/>
+    <workbookView xWindow="0" yWindow="504" windowWidth="16608" windowHeight="9432" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cream Cakes" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="111">
   <si>
     <t>id</t>
   </si>
@@ -341,6 +341,15 @@
   </si>
   <si>
     <t>price charged according to flavour</t>
+  </si>
+  <si>
+    <t>sd4</t>
+  </si>
+  <si>
+    <t>Brownie</t>
+  </si>
+  <si>
+    <t>sweet-delights/brownie.jpeg</t>
   </si>
 </sst>
 </file>
@@ -620,7 +629,7 @@
   </sheetPr>
   <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -1447,10 +1456,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC4"/>
+  <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1581,6 +1590,29 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="2">
+        <v>60</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:H4">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ cakeoclock/cakeoclock.github.io@7339b784543311c02a8eb729dc3d94c608c4e79d 🚀
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="504" windowWidth="16608" windowHeight="9432" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="504" windowWidth="16608" windowHeight="9432"/>
   </bookViews>
   <sheets>
     <sheet name="Cream Cakes" sheetId="1" r:id="rId1"/>
@@ -109,9 +109,6 @@
     <t>Chocolate Cake</t>
   </si>
   <si>
-    <t>cream-cakes/chocolate.jpeg</t>
-  </si>
-  <si>
     <t>cc7</t>
   </si>
   <si>
@@ -133,12 +130,6 @@
     <t>cc9</t>
   </si>
   <si>
-    <t>Mirror Glaze Cake</t>
-  </si>
-  <si>
-    <t>cream-cakes/mirror-glaze.jpeg</t>
-  </si>
-  <si>
     <t>cc10</t>
   </si>
   <si>
@@ -350,6 +341,15 @@
   </si>
   <si>
     <t>sweet-delights/brownie.jpeg</t>
+  </si>
+  <si>
+    <t>dark chocolate cake</t>
+  </si>
+  <si>
+    <t>cream-cakes/blueberry (3)</t>
+  </si>
+  <si>
+    <t>cream-cakes/chocolate</t>
   </si>
 </sst>
 </file>
@@ -629,8 +629,8 @@
   </sheetPr>
   <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -709,7 +709,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>14</v>
@@ -735,7 +735,7 @@
         <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>14</v>
@@ -761,7 +761,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>14</v>
@@ -787,7 +787,7 @@
         <v>13</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>14</v>
@@ -813,7 +813,7 @@
         <v>13</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>14</v>
@@ -830,16 +830,16 @@
         <v>29</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>30</v>
+        <v>109</v>
       </c>
       <c r="D7" s="2">
-        <v>400</v>
+        <v>350</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>14</v>
@@ -850,13 +850,13 @@
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D8" s="2">
         <v>400</v>
@@ -865,7 +865,7 @@
         <v>13</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>14</v>
@@ -876,13 +876,13 @@
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="D9" s="2">
         <v>400</v>
@@ -891,7 +891,7 @@
         <v>13</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>14</v>
@@ -902,13 +902,13 @@
     </row>
     <row r="10" spans="1:29" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="D10" s="2">
         <v>400</v>
@@ -917,7 +917,7 @@
         <v>13</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>14</v>
@@ -928,13 +928,13 @@
     </row>
     <row r="11" spans="1:29" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D11" s="2">
         <v>450</v>
@@ -943,7 +943,7 @@
         <v>13</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>14</v>
@@ -954,13 +954,13 @@
     </row>
     <row r="12" spans="1:29" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D12" s="2">
         <v>500</v>
@@ -969,7 +969,7 @@
         <v>13</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>14</v>
@@ -980,22 +980,22 @@
     </row>
     <row r="13" spans="1:29" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="2">
+        <v>750</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="2">
-        <v>800</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="F13" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>14</v>
@@ -1090,13 +1090,13 @@
     </row>
     <row r="2" spans="1:29" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D2" s="2">
         <v>300</v>
@@ -1105,7 +1105,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>14</v>
@@ -1116,13 +1116,13 @@
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D3" s="2">
         <v>200</v>
@@ -1131,7 +1131,7 @@
         <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>14</v>
@@ -1142,13 +1142,13 @@
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D4" s="2">
         <v>250</v>
@@ -1157,7 +1157,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>14</v>
@@ -1248,19 +1248,19 @@
     </row>
     <row r="2" spans="1:29" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2">
         <v>60</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
@@ -1272,19 +1272,19 @@
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D3" s="2">
         <v>65</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
@@ -1296,19 +1296,19 @@
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D4" s="2">
         <v>65</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
@@ -1320,19 +1320,19 @@
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D5" s="2">
         <v>65</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
@@ -1344,19 +1344,19 @@
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D6" s="2">
         <v>70</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
@@ -1368,19 +1368,19 @@
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D7" s="2">
         <v>80</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
@@ -1392,19 +1392,19 @@
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D8" s="2">
         <v>75</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
@@ -1416,19 +1416,19 @@
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D9" s="2">
         <v>80</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
@@ -1458,7 +1458,7 @@
   </sheetPr>
   <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -1520,19 +1520,19 @@
     </row>
     <row r="2" spans="1:29" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D2" s="2">
         <v>35</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
@@ -1544,19 +1544,19 @@
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D3" s="2">
         <v>45</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
@@ -1568,19 +1568,19 @@
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D4" s="2">
         <v>25</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
@@ -1592,19 +1592,19 @@
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D5" s="2">
         <v>60</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ cakeoclock/cakeoclock.github.io@81ba43aeff1726b9595b0103279e406b0dd71163 🚀
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -346,10 +346,10 @@
     <t>dark chocolate cake</t>
   </si>
   <si>
-    <t>cream-cakes/blueberry (3)</t>
-  </si>
-  <si>
-    <t>cream-cakes/chocolate</t>
+    <t>cream-cakes/chocolate.jpeg</t>
+  </si>
+  <si>
+    <t>cream-cakes/blueberry (3).jpeg</t>
   </si>
 </sst>
 </file>
@@ -630,7 +630,7 @@
   <dimension ref="A1:AC13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -830,7 +830,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D7" s="2">
         <v>350</v>
@@ -908,7 +908,7 @@
         <v>108</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D10" s="2">
         <v>400</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ cakeoclock/cakeoclock.github.io@f1db9d991a2cf96e3bec3ead477f06c0df18f320 🚀
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -343,13 +343,13 @@
     <t>sweet-delights/brownie.jpeg</t>
   </si>
   <si>
-    <t>dark chocolate cake</t>
-  </si>
-  <si>
     <t>cream-cakes/chocolate.jpeg</t>
   </si>
   <si>
-    <t>cream-cakes/blueberry (3).jpeg</t>
+    <t>Dark chocolate cake</t>
+  </si>
+  <si>
+    <t>cream-cakes/blueberry (3).jpg</t>
   </si>
 </sst>
 </file>
@@ -630,7 +630,7 @@
   <dimension ref="A1:AC13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -905,10 +905,10 @@
         <v>36</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="D10" s="2">
         <v>400</v>
@@ -1459,7 +1459,7 @@
   <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ cakeoclock/cakeoclock.github.io@b4d660461e24d11525176820c37ffb8c4bffd166 🚀
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="504" windowWidth="16608" windowHeight="9432"/>
+    <workbookView xWindow="0" yWindow="504" windowWidth="16608" windowHeight="9432" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cream Cakes" sheetId="1" r:id="rId1"/>
@@ -629,7 +629,7 @@
   </sheetPr>
   <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1186,8 +1186,8 @@
   </sheetPr>
   <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1257,7 +1257,7 @@
         <v>58</v>
       </c>
       <c r="D2" s="2">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>59</v>
@@ -1281,7 +1281,7 @@
         <v>62</v>
       </c>
       <c r="D3" s="2">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>59</v>
@@ -1305,7 +1305,7 @@
         <v>65</v>
       </c>
       <c r="D4" s="2">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>59</v>
@@ -1329,7 +1329,7 @@
         <v>68</v>
       </c>
       <c r="D5" s="2">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>59</v>
@@ -1353,7 +1353,7 @@
         <v>71</v>
       </c>
       <c r="D6" s="2">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>59</v>
@@ -1377,7 +1377,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="2">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>59</v>
@@ -1401,7 +1401,7 @@
         <v>77</v>
       </c>
       <c r="D8" s="2">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>59</v>
@@ -1425,7 +1425,7 @@
         <v>80</v>
       </c>
       <c r="D9" s="2">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ cakeoclock/cakeoclock.github.io@8dcc3618ce2595ed5ca0796694774ee1a9334023 🚀
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="504" windowWidth="16608" windowHeight="9432" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="504" windowWidth="16608" windowHeight="9432" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cream Cakes" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="127">
   <si>
     <t>id</t>
   </si>
@@ -350,6 +350,54 @@
   </si>
   <si>
     <t>cream-cakes/blueberry (3).jpg</t>
+  </si>
+  <si>
+    <t>sd5</t>
+  </si>
+  <si>
+    <t>jeera cookies</t>
+  </si>
+  <si>
+    <t>For 100 gm</t>
+  </si>
+  <si>
+    <t>sd6</t>
+  </si>
+  <si>
+    <t>sd7</t>
+  </si>
+  <si>
+    <t>sd8</t>
+  </si>
+  <si>
+    <t>atta cookies</t>
+  </si>
+  <si>
+    <t>chocolate cookies</t>
+  </si>
+  <si>
+    <t>coconut cookies</t>
+  </si>
+  <si>
+    <t>sd9</t>
+  </si>
+  <si>
+    <t>ragi oats cookies</t>
+  </si>
+  <si>
+    <t>sweet-delights/atta-cookies.jpg</t>
+  </si>
+  <si>
+    <t>sweet-delights/chocolate-cookies.jpg</t>
+  </si>
+  <si>
+    <t>sweet-delights/coconut-cookies.jpg</t>
+  </si>
+  <si>
+    <t>sweet-delights/ragi-oats-cookies.jpg</t>
+  </si>
+  <si>
+    <t>sweet-delights/jeera-cookies.jpg</t>
   </si>
 </sst>
 </file>
@@ -630,7 +678,7 @@
   <dimension ref="A1:AC13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -963,7 +1011,7 @@
         <v>42</v>
       </c>
       <c r="D12" s="2">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>13</v>
@@ -1186,7 +1234,7 @@
   </sheetPr>
   <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1456,10 +1504,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC5"/>
+  <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1553,7 +1601,7 @@
         <v>86</v>
       </c>
       <c r="D3" s="2">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>59</v>
@@ -1610,6 +1658,121 @@
         <v>14</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="2">
+        <v>30</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="2">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="2">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="2">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" s="2">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>113</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ cakeoclock/cakeoclock.github.io@8093d30c8a9627c42dd6b99fe56c2d0b8c80e2f4 🚀
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="504" windowWidth="16608" windowHeight="9432" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="504" windowWidth="16608" windowHeight="9432" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cream Cakes" sheetId="1" r:id="rId1"/>
@@ -1234,8 +1234,8 @@
   </sheetPr>
   <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1305,7 +1305,7 @@
         <v>58</v>
       </c>
       <c r="D2" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>59</v>
@@ -1329,7 +1329,7 @@
         <v>62</v>
       </c>
       <c r="D3" s="2">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>59</v>
@@ -1353,7 +1353,7 @@
         <v>65</v>
       </c>
       <c r="D4" s="2">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>59</v>
@@ -1377,7 +1377,7 @@
         <v>68</v>
       </c>
       <c r="D5" s="2">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>59</v>
@@ -1408,7 +1408,7 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>15</v>
@@ -1425,7 +1425,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="2">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>59</v>
@@ -1449,7 +1449,7 @@
         <v>77</v>
       </c>
       <c r="D8" s="2">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>59</v>
@@ -1473,7 +1473,7 @@
         <v>80</v>
       </c>
       <c r="D9" s="2">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>59</v>
@@ -1506,7 +1506,7 @@
   </sheetPr>
   <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ cakeoclock/cakeoclock.github.io@4c235f96b82922017472acfde11797a75e18e8f3 🚀
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="504" windowWidth="16608" windowHeight="9432" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="504" windowWidth="16608" windowHeight="9432" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cream Cakes" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="158">
   <si>
     <t>id</t>
   </si>
@@ -58,9 +58,6 @@
     <t>cream-cakes/vanilla.jpeg</t>
   </si>
   <si>
-    <t>For every 500 gm</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -157,9 +154,6 @@
     <t>cream-cakes/doll.jpeg</t>
   </si>
   <si>
-    <t>For 1 kg</t>
-  </si>
-  <si>
     <t>dc1</t>
   </si>
   <si>
@@ -172,9 +166,6 @@
     <t>dc2</t>
   </si>
   <si>
-    <t>Fruit Cake</t>
-  </si>
-  <si>
     <t>dry-cakes/fruit.jpeg</t>
   </si>
   <si>
@@ -298,42 +289,15 @@
     <t>The evergreen pineapple cake with rich pineapple flavour and delicious cream, makes this one a delicious for all your special occasions.</t>
   </si>
   <si>
-    <t>An all time favourite cake with chocolate cream inside and a crunch of choco chips.</t>
-  </si>
-  <si>
-    <t>Layers of chocolate cake filled with soft and fluffy oreo rich cream with small chunks of oreo biscuit inside.</t>
-  </si>
-  <si>
-    <t>Rich and decadent, this black forest cake is a chocolate lovers delight with a layer of soft and moist chocolate sponge, whipped cream, juicy cherries, and chocolate shavings.</t>
-  </si>
-  <si>
-    <t>A must have cake for the special ones on special ocassions. Filled with rich chocolate cream inside with a top coating of delicious chocolate ganache.</t>
-  </si>
-  <si>
-    <t>Soft and rich red velvet cake with luscious cheese cream and filled with choco chips and cherries.</t>
-  </si>
-  <si>
-    <t>Rich and decadent, this chocolate cake is a dream come true for chocolate lovers with dense but silky smooth chocolate ganache makes this cake a show stopper for all your occasions.</t>
-  </si>
-  <si>
     <t>[Veg preparation] A delicious and rich cake with full of nuts and berries. A healthier version of all cakes with low sugar content. Rum is replace with fruit juices.</t>
   </si>
   <si>
-    <t>A favourite tea time cake with a light crunch of tooti-fruti inside with a light topping of dry fruits.</t>
-  </si>
-  <si>
-    <t>A dry version of the chocolate cake with rich taste of cocoa and nuts. An all time favourite.</t>
-  </si>
-  <si>
     <t>This cake is unique in itself. It has a tangy taste of blueberry with a blueberry filling inside. Fit for any occasion.</t>
   </si>
   <si>
     <t>Representing the sweetness and joy of life, this cake is one of the favourites of children and has rich flavours of strawberry.</t>
   </si>
   <si>
-    <t>price charged according to flavour</t>
-  </si>
-  <si>
     <t>sd4</t>
   </si>
   <si>
@@ -355,9 +319,6 @@
     <t>sd5</t>
   </si>
   <si>
-    <t>jeera cookies</t>
-  </si>
-  <si>
     <t>For 100 gm</t>
   </si>
   <si>
@@ -370,21 +331,9 @@
     <t>sd8</t>
   </si>
   <si>
-    <t>atta cookies</t>
-  </si>
-  <si>
-    <t>chocolate cookies</t>
-  </si>
-  <si>
-    <t>coconut cookies</t>
-  </si>
-  <si>
     <t>sd9</t>
   </si>
   <si>
-    <t>ragi oats cookies</t>
-  </si>
-  <si>
     <t>sweet-delights/atta-cookies.jpg</t>
   </si>
   <si>
@@ -398,6 +347,150 @@
   </si>
   <si>
     <t>sweet-delights/jeera-cookies.jpg</t>
+  </si>
+  <si>
+    <t>Jeera cookies</t>
+  </si>
+  <si>
+    <t>Atta cookies</t>
+  </si>
+  <si>
+    <t>Chocolate cookies</t>
+  </si>
+  <si>
+    <t>Coconut cookies</t>
+  </si>
+  <si>
+    <t>Ragi oats cookies</t>
+  </si>
+  <si>
+    <t>cc13</t>
+  </si>
+  <si>
+    <t>Opera Cake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cc14 </t>
+  </si>
+  <si>
+    <t>Orange Cake</t>
+  </si>
+  <si>
+    <t>Rabdi Cake</t>
+  </si>
+  <si>
+    <t>cc15</t>
+  </si>
+  <si>
+    <t>cc16</t>
+  </si>
+  <si>
+    <t>Rasmalai Cake</t>
+  </si>
+  <si>
+    <t>Mango Cake</t>
+  </si>
+  <si>
+    <t>cc17</t>
+  </si>
+  <si>
+    <t>cc18</t>
+  </si>
+  <si>
+    <t>Mud Cake</t>
+  </si>
+  <si>
+    <t>Gulab Jamun Cake</t>
+  </si>
+  <si>
+    <t>Lemon Mousse Cake</t>
+  </si>
+  <si>
+    <t>cc19</t>
+  </si>
+  <si>
+    <t>cc20</t>
+  </si>
+  <si>
+    <t>Vanilla Fruit Cake</t>
+  </si>
+  <si>
+    <t>Orange Fruit Cake</t>
+  </si>
+  <si>
+    <t>dc4</t>
+  </si>
+  <si>
+    <t>dc5</t>
+  </si>
+  <si>
+    <t>dc6</t>
+  </si>
+  <si>
+    <t>Walnut Dates Cake</t>
+  </si>
+  <si>
+    <t>Suji Cake</t>
+  </si>
+  <si>
+    <t>[Veg preparation] A favourite tea time cake with a light crunch of tutti-fruti .</t>
+  </si>
+  <si>
+    <t>[Veg preparation] A dry version of the chocolate cake with rich taste of cocoa and nuts. An all time favourite.</t>
+  </si>
+  <si>
+    <t>[Veg preparation] Orange flavoured cake with tutti-frutti.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Veg preparation] </t>
+  </si>
+  <si>
+    <t>[Veg preparation] Super tasty and healthy,no maida cake with dry fruits.</t>
+  </si>
+  <si>
+    <t>[Veg preparation] An all time favourite cake with chocolate cream inside and a crunch of choco chips.</t>
+  </si>
+  <si>
+    <t>[Veg preparation] Layers of chocolate cake filled with soft and fluffy oreo rich cream with small chunks of oreo biscuit inside.</t>
+  </si>
+  <si>
+    <t>[Veg preparation] Rich and decadent, this black forest cake is a chocolate lovers delight with a layer of soft and moist chocolate sponge, whipped cream, juicy cherries, and chocolate shavings.</t>
+  </si>
+  <si>
+    <t>[Veg preparation] A must have cake for the special ones on special ocassions. Filled with rich chocolate cream inside with a top coating of delicious chocolate ganache.</t>
+  </si>
+  <si>
+    <t>[Veg preparation] Rich and decadent, this chocolate cake is a dream come true for chocolate lovers with dense but silky smooth chocolate ganache makes this cake a show stopper for all your occasions.</t>
+  </si>
+  <si>
+    <t>[Veg preparation] Soft and rich red velvet cake with luscious cheese cream and filled with choco chips and cherries.</t>
+  </si>
+  <si>
+    <t>[Veg preparation] price charged according to flavour</t>
+  </si>
+  <si>
+    <t>[Veg preparation] A rich coffe flavoued cake.</t>
+  </si>
+  <si>
+    <t>[Veg preparation] No maida cake with walnuts and dates.(Available with sugar/without sugar only using dates ).</t>
+  </si>
+  <si>
+    <t>Banana Cake</t>
+  </si>
+  <si>
+    <t>[Veg preparation]</t>
+  </si>
+  <si>
+    <t>[Veg preparation]A super healthy and delicious cake made with chocolate,banana,oats,aata and NO MAIDA.</t>
+  </si>
+  <si>
+    <t>Oats Aata Banana Cake</t>
+  </si>
+  <si>
+    <t>dc7</t>
+  </si>
+  <si>
+    <t>dc8</t>
   </si>
 </sst>
 </file>
@@ -675,10 +768,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC13"/>
+  <dimension ref="A1:AC21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -750,306 +843,405 @@
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2">
-        <v>300</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2">
-        <v>350</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2">
-        <v>350</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="2">
-        <v>350</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="2">
-        <v>350</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D7" s="2">
-        <v>350</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>93</v>
+        <v>143</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="2">
-        <v>400</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>94</v>
+        <v>144</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="2">
-        <v>400</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D10" s="2">
-        <v>400</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>96</v>
+        <v>146</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="2">
-        <v>450</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="2">
-        <v>450</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>97</v>
+        <v>148</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="2">
-        <v>750</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>104</v>
+        <v>149</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" t="s">
+        <v>150</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" t="s">
+        <v>141</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="F17" t="s">
+        <v>141</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A18" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="F18" t="s">
+        <v>141</v>
+      </c>
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A19" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="F19" t="s">
+        <v>141</v>
+      </c>
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="F20" t="s">
+        <v>141</v>
+      </c>
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A21" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="F21" t="s">
+        <v>141</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1073,10 +1265,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC4"/>
+  <dimension ref="A1:AC14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1138,88 +1330,179 @@
     </row>
     <row r="2" spans="1:29" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="2">
-        <v>300</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>51</v>
+        <v>131</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="2">
-        <v>200</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>100</v>
+        <v>138</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="2">
-        <v>250</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>101</v>
+        <v>139</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" t="s">
+        <v>151</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F8" t="s">
+        <v>153</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F9" t="s">
+        <v>154</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="15.75" customHeight="1">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:29" ht="15.75" customHeight="1">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:29" ht="15.75" customHeight="1">
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:29" ht="15.75" customHeight="1">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:29" ht="15.75" customHeight="1">
+      <c r="B14" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:H4">
       <formula1>"yes,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E4">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E7">
       <formula1>"For every 500 gm,Per Piece"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1234,8 +1517,8 @@
   </sheetPr>
   <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1296,194 +1579,162 @@
     </row>
     <row r="2" spans="1:29" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="2">
-        <v>40</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>59</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="2">
-        <v>45</v>
-      </c>
-      <c r="E3" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="2">
-        <v>45</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>59</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="2">
-        <v>45</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>59</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="2">
-        <v>60</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>59</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="2">
-        <v>60</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>59</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="2">
-        <v>55</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>59</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="2">
-        <v>60</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>59</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1506,8 +1757,8 @@
   </sheetPr>
   <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1568,212 +1819,212 @@
     </row>
     <row r="2" spans="1:29" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D2" s="2">
         <v>35</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D3" s="2">
         <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D4" s="2">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D5" s="2">
         <v>60</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="D6" s="2">
         <v>30</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C7" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="D7" s="2">
         <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C8" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="D8" s="2">
         <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C9" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="D9" s="2">
         <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C10" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="D10" s="2">
         <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ cakeoclock/cakeoclock.github.io@56936c02b89b75d9c598ee592ea17ca5f3e6e3ee 🚀
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="504" windowWidth="16608" windowHeight="9432" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="504" windowWidth="16608" windowHeight="9432" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cream Cakes" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="173">
   <si>
     <t>id</t>
   </si>
@@ -491,6 +491,51 @@
   </si>
   <si>
     <t>dc8</t>
+  </si>
+  <si>
+    <t>New York Cheesecake</t>
+  </si>
+  <si>
+    <t>Lemon  Cheesecake</t>
+  </si>
+  <si>
+    <t>Strawberry  Cheesecake</t>
+  </si>
+  <si>
+    <t>Blueberry  Cheesecake</t>
+  </si>
+  <si>
+    <t>Biscoff  Cheesecake</t>
+  </si>
+  <si>
+    <t>dc9</t>
+  </si>
+  <si>
+    <t>dc10</t>
+  </si>
+  <si>
+    <t>dc11</t>
+  </si>
+  <si>
+    <t>dc12</t>
+  </si>
+  <si>
+    <t>dc13</t>
+  </si>
+  <si>
+    <t>dry-cakes/Lemon-Cheesecake.jpg</t>
+  </si>
+  <si>
+    <t>dry-cakes/Strawberry-Cheesecake.jpg</t>
+  </si>
+  <si>
+    <t>dry-cakes/Blueberry-Cheesecake.jpg</t>
+  </si>
+  <si>
+    <t>dry-cakes/Biscoff-Cheesecake.jpg</t>
+  </si>
+  <si>
+    <t>dry-cakes/New-York-Cheesecake.jpg</t>
   </si>
 </sst>
 </file>
@@ -1267,8 +1312,8 @@
   </sheetPr>
   <dimension ref="A1:AC14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1483,19 +1528,104 @@
       </c>
     </row>
     <row r="10" spans="1:29" ht="15.75" customHeight="1">
-      <c r="B10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" t="s">
+        <v>172</v>
+      </c>
+      <c r="F10" t="s">
+        <v>153</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:29" ht="15.75" customHeight="1">
-      <c r="B11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:29" ht="15.75" customHeight="1">
-      <c r="B12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" t="s">
+        <v>169</v>
+      </c>
+      <c r="F12" t="s">
+        <v>153</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:29" ht="15.75" customHeight="1">
-      <c r="B13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" t="s">
+        <v>170</v>
+      </c>
+      <c r="F13" t="s">
+        <v>153</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="1:29" ht="15.75" customHeight="1">
-      <c r="B14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" t="s">
+        <v>171</v>
+      </c>
+      <c r="F14" t="s">
+        <v>153</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -1757,7 +1887,7 @@
   </sheetPr>
   <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>